<commit_message>
Section layout, footer and home
Section layout, footer and home
</commit_message>
<xml_diff>
--- a/ProjectMarkingScheme.xlsx
+++ b/ProjectMarkingScheme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardo/Desktop/NBCC/1T_Responsive Web Design_1219-2656/Term Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardo/Desktop/NBCC/1T_Responsive Web Design_1219-2656/Term Project/Phase 2 - Website/RWD-FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08F1F88-7DB9-B248-BC40-9E20ED8D89E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A70658-9587-8642-B44B-153E5E0DC614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{720EC24C-AFDA-4AC6-9634-90AAF959B597}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t xml:space="preserve">Navigation Panel </t>
   </si>
@@ -147,43 +147,32 @@
     <t>Overall Quality / Miscellaneous (10%)</t>
   </si>
   <si>
-    <t>inside carousel</t>
-  </si>
-  <si>
-    <t>inside navbar</t>
-  </si>
-  <si>
-    <t>inside video</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>IMPLEMETADO</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>IMPLEMENTADO, AJUSTANDO LAYOUT</t>
-  </si>
-  <si>
     <t>TA TOP PAI</t>
+  </si>
+  <si>
+    <t>Embbeded</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -273,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -292,25 +281,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,33 +633,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2A49CA-B12C-4FB4-8F29-0F08F2E42B92}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -660,7 +667,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>28</v>
@@ -670,164 +677,141 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7">
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="B9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>4</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10">
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12">
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13">
+      <c r="C13" s="8">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C14" s="8">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>33</v>
       </c>
@@ -1041,8 +1025,8 @@
       <c r="C38" s="1">
         <v>10</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>41</v>
+      <c r="D38" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1077,8 +1061,8 @@
       <c r="C42" s="1">
         <v>10</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>46</v>
+      <c r="D42" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
All internal pages created
All internal pages created (History done, Culture ongoing, the others just structured)
</commit_message>
<xml_diff>
--- a/ProjectMarkingScheme.xlsx
+++ b/ProjectMarkingScheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardo/Desktop/NBCC/1T_Responsive Web Design_1219-2656/Term Project/Phase 2 - Website/RWD-FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A70658-9587-8642-B44B-153E5E0DC614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197D2750-769B-C343-A489-2CC79222E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{720EC24C-AFDA-4AC6-9634-90AAF959B597}"/>
+    <workbookView xWindow="-20" yWindow="-21140" windowWidth="25600" windowHeight="20760" xr2:uid="{720EC24C-AFDA-4AC6-9634-90AAF959B597}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t xml:space="preserve">Navigation Panel </t>
   </si>
@@ -75,9 +75,6 @@
     <t xml:space="preserve">Climate </t>
   </si>
   <si>
-    <t xml:space="preserve">Famous Sites </t>
-  </si>
-  <si>
     <t xml:space="preserve">Date and Time </t>
   </si>
   <si>
@@ -150,13 +147,31 @@
     <t>OK</t>
   </si>
   <si>
-    <t>TA TOP PAI</t>
-  </si>
-  <si>
-    <t>Embbeded</t>
-  </si>
-  <si>
-    <t>Y</t>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>IMPLEMETADO</t>
+  </si>
+  <si>
+    <t>ONGOING</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Famous Landmarks &amp; Sites </t>
+  </si>
+  <si>
+    <t>CONTENT</t>
+  </si>
+  <si>
+    <t>PAGE</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Culture</t>
   </si>
 </sst>
 </file>
@@ -262,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -281,43 +296,27 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,193 +632,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2A49CA-B12C-4FB4-8F29-0F08F2E42B92}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>2</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="8">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8">
-        <v>2</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="8">
-        <v>2</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8">
-        <v>2</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>7</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="8">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>8</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="8">
-        <v>2</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>8</v>
@@ -827,9 +832,14 @@
       <c r="C17" s="1">
         <v>2</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -837,9 +847,14 @@
       <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>10</v>
@@ -847,9 +862,14 @@
       <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>11</v>
@@ -857,9 +877,14 @@
       <c r="C20" s="1">
         <v>2</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>12</v>
@@ -867,213 +892,269 @@
       <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
+      <c r="B22" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D22" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
       </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1">
         <v>4</v>
       </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D31" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1">
         <v>4</v>
       </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D32" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1">
         <v>4</v>
       </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D33" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1">
         <v>4</v>
       </c>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D34" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="1">
         <v>4</v>
       </c>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D35" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" s="1">
         <v>10</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D38" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="1">
         <v>10</v>
       </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D39" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="1">
         <v>10</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2">
@@ -1081,7 +1162,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Final version - All pages completed
Final version - All pages completed
</commit_message>
<xml_diff>
--- a/ProjectMarkingScheme.xlsx
+++ b/ProjectMarkingScheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardo/Desktop/NBCC/1T_Responsive Web Design_1219-2656/Term Project/Phase 2 - Website/RWD-FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197D2750-769B-C343-A489-2CC79222E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26327B38-3793-4E4B-86BF-470A9ACDF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-21140" windowWidth="25600" windowHeight="20760" xr2:uid="{720EC24C-AFDA-4AC6-9634-90AAF959B597}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{720EC24C-AFDA-4AC6-9634-90AAF959B597}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
   <si>
     <t xml:space="preserve">Navigation Panel </t>
   </si>
@@ -151,12 +151,6 @@
   </si>
   <si>
     <t>IMPLEMETADO</t>
-  </si>
-  <si>
-    <t>ONGOING</t>
-  </si>
-  <si>
-    <t>NOK</t>
   </si>
   <si>
     <t xml:space="preserve">Famous Landmarks &amp; Sites </t>
@@ -245,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,12 +255,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,19 +289,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -635,7 +622,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="D27" sqref="D27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -647,11 +634,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -818,10 +805,10 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -850,8 +837,8 @@
       <c r="D18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>39</v>
+      <c r="E18" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -865,8 +852,8 @@
       <c r="D19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>39</v>
+      <c r="E19" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -877,11 +864,11 @@
       <c r="C20" s="1">
         <v>2</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>39</v>
+      <c r="D20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -895,14 +882,14 @@
       <c r="D21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>39</v>
+      <c r="E21" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -910,8 +897,8 @@
       <c r="D22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>39</v>
+      <c r="E22" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -922,11 +909,11 @@
       <c r="C23" s="1">
         <v>2</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>39</v>
+      <c r="D23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -940,8 +927,8 @@
       <c r="D24" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>39</v>
+      <c r="E24" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -955,8 +942,8 @@
       <c r="D25" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="9" t="s">
-        <v>39</v>
+      <c r="E25" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -970,8 +957,8 @@
       <c r="D26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>39</v>
+      <c r="E26" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -982,11 +969,11 @@
       <c r="C27" s="1">
         <v>2</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>39</v>
+      <c r="D27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -997,11 +984,11 @@
       <c r="C28" s="1">
         <v>2</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>39</v>
+      <c r="D28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1066,7 +1053,7 @@
         <v>36</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1081,7 +1068,7 @@
         <v>36</v>
       </c>
       <c r="E35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">

</xml_diff>